<commit_message>
Smart-Contract Timeline Update 1.5
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -53,8 +53,9 @@
     <t>Monday</t>
   </si>
   <si>
-    <t xml:space="preserve">Updated Demo_2.html to represent timeline sketch 3.0
-</t>
+    <t>▫ Updated Demo_2.html to represent timeline sketch 3.0
+▫ Seperated internal style sheets into external ones
+▫ Need to fix issues with wonky resizing -- May look weird on other screen ratios.</t>
   </si>
 </sst>
 </file>
@@ -447,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,10 +553,20 @@
     </row>
     <row r="9" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="4"/>
+      <c r="F9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="H9" s="1">
+        <v>3</v>
+      </c>
       <c r="J9" s="6"/>
     </row>
     <row r="10" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="4"/>
+      <c r="J10" s="6"/>
     </row>
     <row r="11" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="4"/>
@@ -679,7 +690,6 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="J8:J9"/>
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:J6"/>
@@ -690,6 +700,7 @@
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="G5:G6"/>
+    <mergeCell ref="J8:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Smart-Contract Timeline Update 1.6
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -53,9 +53,20 @@
     <t>Monday</t>
   </si>
   <si>
-    <t>▫ Updated Demo_2.html to represent timeline sketch 3.0
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">▫ Updated Demo_2.html to represent timeline sketch 3.0
 ▫ Seperated internal style sheets into external ones
-▫ Need to fix issues with wonky resizing -- May look weird on other screen ratios.</t>
+▫ Need to fix issues with wonky resizing -- May look weird on other screen ratios.
+</t>
+  </si>
+  <si>
+    <t>▫ Adjusted Demo to specifications
+▫ Added Filter Functionality Design</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
   </si>
 </sst>
 </file>
@@ -97,7 +108,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="7"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -133,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="18" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -142,29 +153,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -446,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J50"/>
+  <dimension ref="B2:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,132 +486,167 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="7" t="s">
+      <c r="E5" s="8"/>
+      <c r="F5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="7" t="s">
+      <c r="I5" s="8"/>
+      <c r="J5" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="8"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="7"/>
     </row>
     <row r="7" spans="2:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="4"/>
     </row>
     <row r="8" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4">
+        <v>43305</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>3</v>
+      </c>
+      <c r="C9" s="4">
+        <v>43304</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>2</v>
+      </c>
+      <c r="C10" s="4">
+        <v>43300</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H10" s="1">
+        <v>4</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="13">
         <v>1</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C11" s="14">
         <v>43297</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="H11" s="1">
+        <v>3</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="13"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="13"/>
+      <c r="F12" s="2">
         <v>0.33333333333333331</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G12" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H12" s="1">
         <v>3</v>
       </c>
-      <c r="J8" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="4"/>
-      <c r="F9" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0.625</v>
-      </c>
-      <c r="H9" s="1">
-        <v>3</v>
-      </c>
-      <c r="J9" s="6"/>
-    </row>
-    <row r="10" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="4"/>
-      <c r="J10" s="6"/>
-    </row>
-    <row r="11" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="4"/>
+      <c r="J12" s="16"/>
     </row>
     <row r="13" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="4"/>
-    </row>
+    <row r="14" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="3:3" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="3:3" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="4"/>
-    </row>
+    <row r="18" spans="3:3" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="3:3" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="4"/>
     </row>
@@ -688,8 +743,11 @@
     <row r="50" spans="3:3" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C50" s="4"/>
     </row>
+    <row r="51" spans="3:3" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C51" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="14">
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:J6"/>
@@ -700,7 +758,10 @@
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="G5:G6"/>
-    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="J11:J12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Aion Announcement Header Update 1.0
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Tuesday</t>
+  </si>
+  <si>
+    <t>▫ Created Aion Announcement Header</t>
   </si>
 </sst>
 </file>
@@ -153,6 +156,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -179,9 +185,6 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -469,7 +472,7 @@
   <dimension ref="B2:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,94 +489,90 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="6" t="s">
+      <c r="E5" s="9"/>
+      <c r="F5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="6" t="s">
+      <c r="I5" s="9"/>
+      <c r="J5" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="7"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="8"/>
     </row>
     <row r="7" spans="2:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="1">
-        <v>4</v>
-      </c>
-      <c r="C8" s="4">
-        <v>43305</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0.45833333333333331</v>
-      </c>
-    </row>
+    <row r="8" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C9" s="4">
-        <v>43304</v>
+        <v>43305</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F9" s="2">
-        <v>0.625</v>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H9" s="1">
+        <v>2</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -595,18 +594,18 @@
       <c r="H10" s="1">
         <v>4</v>
       </c>
-      <c r="J10" s="15" t="s">
+      <c r="J10" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="13">
+      <c r="B11" s="14">
         <v>1</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="15">
         <v>43297</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="14" t="s">
         <v>8</v>
       </c>
       <c r="F11" s="2">
@@ -623,9 +622,9 @@
       </c>
     </row>
     <row r="12" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="13"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="14"/>
       <c r="F12" s="2">
         <v>0.33333333333333331</v>
       </c>
@@ -748,6 +747,10 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="J11:J12"/>
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:J6"/>
@@ -758,10 +761,6 @@
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="G5:G6"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="J11:J12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Social Media Branding Update 1.0
</commit_message>
<xml_diff>
--- a/Time Log.xlsx
+++ b/Time Log.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>▫ Created Aion Announcement Header</t>
+  </si>
+  <si>
+    <t>▫ Created PNG/JPG Amberdata Logo icons in 8 different sizes</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>▫ Created graphics for social media headers</t>
+  </si>
+  <si>
+    <t>▫ Contiued editing graphics for social media headers</t>
   </si>
 </sst>
 </file>
@@ -159,6 +171,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -179,15 +200,6 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -469,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J51"/>
+  <dimension ref="B2:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,169 +501,225 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="7" t="s">
+      <c r="E5" s="12"/>
+      <c r="F5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="7" t="s">
+      <c r="I5" s="12"/>
+      <c r="J5" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="8"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="11"/>
     </row>
     <row r="7" spans="2:10" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4">
+        <v>43307</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H8" s="1">
+        <v>3</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="9" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>4</v>
       </c>
       <c r="C9" s="4">
-        <v>43305</v>
+        <v>43306</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F9" s="2">
-        <v>0.58333333333333337</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="G9" s="2">
-        <v>0.66666666666666663</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="H9" s="1">
         <v>2</v>
       </c>
       <c r="J9" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="7">
+        <v>3</v>
+      </c>
+      <c r="C10" s="8">
+        <v>43305</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="7"/>
+      <c r="F11" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H11" s="1">
+        <v>2</v>
+      </c>
+      <c r="J11" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="1">
+    <row r="12" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
         <v>2</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C12" s="4">
         <v>43300</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F12" s="2">
         <v>0.5</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G12" s="2">
         <v>0.66666666666666663</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H12" s="1">
         <v>4</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="J12" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="14">
+    <row r="13" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="7">
         <v>1</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C13" s="8">
         <v>43297</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D13" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F13" s="2">
         <v>0.5</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G13" s="2">
         <v>0.625</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H13" s="1">
         <v>3</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="J13" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="14"/>
-      <c r="F12" s="2">
+    <row r="14" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="7"/>
+      <c r="F14" s="2">
         <v>0.33333333333333331</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G14" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H14" s="1">
         <v>3</v>
       </c>
-      <c r="J12" s="16"/>
-    </row>
-    <row r="13" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="4"/>
+    </row>
     <row r="16" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="3:3" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="4"/>
-    </row>
+    <row r="17" spans="3:3" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="3:3" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="3:3" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="3:3" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="4"/>
-    </row>
+    <row r="20" spans="3:3" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="3:3" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="4"/>
     </row>
@@ -745,15 +813,14 @@
     <row r="51" spans="3:3" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C51" s="4"/>
     </row>
+    <row r="52" spans="3:3" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C52" s="4"/>
+    </row>
+    <row r="53" spans="3:3" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C53" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
+  <mergeCells count="17">
     <mergeCell ref="B2:J3"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
@@ -761,6 +828,16 @@
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="G5:G6"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B10:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>